<commit_message>
Update experiments results spreadsheet
</commit_message>
<xml_diff>
--- a/data/experiment_results.xlsx
+++ b/data/experiment_results.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28224"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/efeonal/Documents/UU Courses/MethodsInAI/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{28074829-2F78-7041-9297-611AC12D6062}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFFF1531-18AD-4D4E-8308-41E6672B3F92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{39168E71-D0F7-C144-863E-24EADCC3AA9E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
   <si>
     <t>GENDER</t>
   </si>
@@ -68,6 +68,24 @@
     <t>MALE_INTEGRITY</t>
   </si>
   <si>
+    <t>FEMALE_COMPETENCE_N</t>
+  </si>
+  <si>
+    <t>FEMALE_BENEVOLENCE_N</t>
+  </si>
+  <si>
+    <t>FEMALE_INTEGRITY_N</t>
+  </si>
+  <si>
+    <t>MALE_COMPETENCE_N</t>
+  </si>
+  <si>
+    <t>MALE_BENEVOLENCE_N</t>
+  </si>
+  <si>
+    <t>MALE_INTEGRITY_N</t>
+  </si>
+  <si>
     <t>Male</t>
   </si>
   <si>
@@ -75,31 +93,13 @@
   </si>
   <si>
     <t>Female</t>
-  </si>
-  <si>
-    <t>FEMALE_COMPETENCE_N</t>
-  </si>
-  <si>
-    <t>FEMALE_BENEVOLENCE_N</t>
-  </si>
-  <si>
-    <t>FEMALE_INTEGRITY_N</t>
-  </si>
-  <si>
-    <t>MALE_COMPETENCE_N</t>
-  </si>
-  <si>
-    <t>MALE_BENEVOLENCE_N</t>
-  </si>
-  <si>
-    <t>MALE_INTEGRITY_N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -214,10 +214,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF2D46EE-EC83-E445-A494-263D10110AB9}" name="Table1" displayName="Table1" ref="A1:P11" totalsRowCount="1" headerRowDxfId="2">
-  <autoFilter ref="A1:P10" xr:uid="{EF2D46EE-EC83-E445-A494-263D10110AB9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{EF2D46EE-EC83-E445-A494-263D10110AB9}" name="Table1" displayName="Table1" ref="A1:P17" totalsRowCount="1" headerRowDxfId="2">
+  <autoFilter ref="A1:P16" xr:uid="{EF2D46EE-EC83-E445-A494-263D10110AB9}"/>
   <tableColumns count="16">
-    <tableColumn id="1" xr3:uid="{0B0ADC2B-87A6-3640-A11D-641A8F80D4FB}" name="GENDER" dataDxfId="1" totalsRowDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{0B0ADC2B-87A6-3640-A11D-641A8F80D4FB}" name="GENDER" dataDxfId="0" totalsRowDxfId="1"/>
     <tableColumn id="2" xr3:uid="{37ADAA08-F83D-4340-B8F5-F75626BE9EA1}" name="TEXT_COMPETENCE" totalsRowFunction="custom">
       <totalsRowFormula>AVERAGE(Table1[TEXT_COMPETENCE])</totalsRowFormula>
     </tableColumn>
@@ -591,32 +591,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C88E4FC1-B084-8C4E-A9CE-93365B35338A}">
-  <dimension ref="A1:S11"/>
+  <dimension ref="A1:S17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.95"/>
   <cols>
-    <col min="2" max="2" width="19.83203125" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.875" customWidth="1"/>
+    <col min="3" max="3" width="20.625" customWidth="1"/>
     <col min="4" max="4" width="16.5" customWidth="1"/>
-    <col min="5" max="5" width="22.83203125" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.875" customWidth="1"/>
+    <col min="6" max="6" width="23.625" customWidth="1"/>
     <col min="7" max="7" width="19.5" customWidth="1"/>
-    <col min="8" max="8" width="20.83203125" customWidth="1"/>
-    <col min="9" max="9" width="21.6640625" customWidth="1"/>
+    <col min="8" max="8" width="20.875" customWidth="1"/>
+    <col min="9" max="9" width="21.625" customWidth="1"/>
     <col min="10" max="10" width="17.5" customWidth="1"/>
     <col min="11" max="11" width="25" customWidth="1"/>
-    <col min="12" max="12" width="25.83203125" customWidth="1"/>
-    <col min="13" max="13" width="21.6640625" customWidth="1"/>
+    <col min="12" max="12" width="25.875" customWidth="1"/>
+    <col min="13" max="13" width="21.625" customWidth="1"/>
     <col min="14" max="14" width="23" customWidth="1"/>
-    <col min="15" max="15" width="23.83203125" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
+    <col min="15" max="15" width="23.875" customWidth="1"/>
+    <col min="16" max="16" width="19.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -648,30 +648,30 @@
         <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>18</v>
       </c>
       <c r="Q1" s="1"/>
       <c r="R1" s="1"/>
       <c r="S1" s="1"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19">
       <c r="A2" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B2">
         <v>3</v>
@@ -725,9 +725,9 @@
         <v>-2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19">
       <c r="A3" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B3">
         <v>6</v>
@@ -781,9 +781,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19">
       <c r="A4" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -837,9 +837,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19">
       <c r="A5" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -893,9 +893,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19">
       <c r="A6" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -949,9 +949,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1005,9 +1005,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -1061,9 +1061,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="B9">
         <v>7</v>
@@ -1117,9 +1117,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19">
       <c r="A10" s="2" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>9</v>
@@ -1173,71 +1173,407 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A11" s="2"/>
+    <row r="11" spans="1:19">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11">
+        <v>3</v>
+      </c>
+      <c r="D11">
+        <v>7</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="G11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>3</v>
+      </c>
+      <c r="J11">
+        <v>7</v>
+      </c>
+      <c r="K11">
+        <f>E11-$B11</f>
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <f>F11-$C11</f>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <f>G11-$D11</f>
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <f>H11-$B11</f>
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>I11-$C11</f>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f>J11-$D11</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" ht="15.75">
+      <c r="A12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12">
+        <v>8</v>
+      </c>
+      <c r="C12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>7</v>
+      </c>
+      <c r="E12">
+        <v>5</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>8</v>
+      </c>
+      <c r="I12">
+        <v>8</v>
+      </c>
+      <c r="J12">
+        <v>7</v>
+      </c>
+      <c r="K12">
+        <f>E12-$B12</f>
+        <v>-3</v>
+      </c>
+      <c r="L12">
+        <f>F12-$C12</f>
+        <v>-2</v>
+      </c>
+      <c r="M12">
+        <f>G12-$D12</f>
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <f>H12-$B12</f>
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>I12-$C12</f>
+        <v>1</v>
+      </c>
+      <c r="P12">
+        <f>J12-$D12</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" ht="15.75">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13">
+        <v>6</v>
+      </c>
+      <c r="D13">
+        <v>10</v>
+      </c>
+      <c r="E13">
+        <v>6</v>
+      </c>
+      <c r="F13">
+        <v>6</v>
+      </c>
+      <c r="G13">
+        <v>10</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13">
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <f>E13-$B13</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>F13-$C13</f>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <f>G13-$D13</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <f>H13-$B13</f>
+        <v>-2</v>
+      </c>
+      <c r="O13">
+        <f>I13-$C13</f>
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <f>J13-$D13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" ht="15.75">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>3</v>
+      </c>
+      <c r="D14">
+        <v>10</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14">
+        <v>10</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>3</v>
+      </c>
+      <c r="J14">
+        <v>10</v>
+      </c>
+      <c r="K14">
+        <f>E14-$B14</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>F14-$C14</f>
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <f>G14-$D14</f>
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <f>H14-$B14</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>I14-$C14</f>
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <f>J14-$D14</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" ht="15.75">
+      <c r="A15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>9</v>
+      </c>
+      <c r="E15">
+        <v>8</v>
+      </c>
+      <c r="F15">
+        <v>9</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>9</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+      <c r="J15">
+        <v>8</v>
+      </c>
+      <c r="K15">
+        <f>E15-$B15</f>
+        <v>1</v>
+      </c>
+      <c r="L15">
+        <f>F15-$C15</f>
+        <v>3</v>
+      </c>
+      <c r="M15">
+        <f>G15-$D15</f>
+        <v>-2</v>
+      </c>
+      <c r="N15">
+        <f>H15-$B15</f>
+        <v>2</v>
+      </c>
+      <c r="O15">
+        <f>I15-$C15</f>
+        <v>1</v>
+      </c>
+      <c r="P15">
+        <f>J15-$D15</f>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:19" ht="15.75">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>6</v>
+      </c>
+      <c r="D16">
+        <v>9</v>
+      </c>
+      <c r="E16">
+        <v>9</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>8</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+      <c r="J16">
+        <v>9</v>
+      </c>
+      <c r="K16">
+        <f>E16-$B16</f>
+        <v>2</v>
+      </c>
+      <c r="L16">
+        <f>F16-$C16</f>
+        <v>3</v>
+      </c>
+      <c r="M16">
+        <f>G16-$D16</f>
+        <v>-2</v>
+      </c>
+      <c r="N16">
+        <f>H16-$B16</f>
+        <v>1</v>
+      </c>
+      <c r="O16">
+        <f>I16-$C16</f>
+        <v>1</v>
+      </c>
+      <c r="P16">
+        <f>J16-$D16</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75">
+      <c r="A17" s="2"/>
+      <c r="B17">
         <f>AVERAGE(Table1[TEXT_COMPETENCE])</f>
-        <v>5.1111111111111107</v>
-      </c>
-      <c r="C11">
+        <v>5.4</v>
+      </c>
+      <c r="C17">
         <f>AVERAGE(Table1[TEXT_BENEVOLENCE])</f>
-        <v>4.8888888888888893</v>
-      </c>
-      <c r="D11">
+        <v>5</v>
+      </c>
+      <c r="D17">
         <f>AVERAGE(Table1[TEXT_INTEGRITY])</f>
-        <v>5.5555555555555554</v>
-      </c>
-      <c r="E11">
+        <v>6.8</v>
+      </c>
+      <c r="E17">
         <f>AVERAGE(Table1[FEMALE_COMPETENCE])</f>
-        <v>6.4444444444444446</v>
-      </c>
-      <c r="F11">
+        <v>6.2</v>
+      </c>
+      <c r="F17">
         <f>AVERAGE(Table1[FEMALE_BENEVOLENCE])</f>
-        <v>6.4444444444444446</v>
-      </c>
-      <c r="G11">
+        <v>6.2</v>
+      </c>
+      <c r="G17">
         <f>AVERAGE(Table1[FEMALE_INTEGRITY])</f>
-        <v>7.5555555555555554</v>
-      </c>
-      <c r="H11">
+        <v>7.7333333333333334</v>
+      </c>
+      <c r="H17">
         <f>AVERAGE(Table1[MALE_COMPETENCE])</f>
         <v>6</v>
       </c>
-      <c r="I11">
+      <c r="I17">
         <f>AVERAGE(Table1[MALE_BENEVOLENCE])</f>
-        <v>6.1111111111111107</v>
-      </c>
-      <c r="J11">
+        <v>5.9333333333333336</v>
+      </c>
+      <c r="J17">
         <f>AVERAGE(Table1[MALE_INTEGRITY])</f>
-        <v>7</v>
-      </c>
-      <c r="K11">
+        <v>7.6</v>
+      </c>
+      <c r="K17">
         <f>AVERAGE(Table1[FEMALE_COMPETENCE_N])</f>
-        <v>1.3333333333333333</v>
-      </c>
-      <c r="L11">
+        <v>0.8</v>
+      </c>
+      <c r="L17">
         <f>AVERAGE(Table1[FEMALE_BENEVOLENCE_N])</f>
-        <v>1.5555555555555556</v>
-      </c>
-      <c r="M11">
+        <v>1.2</v>
+      </c>
+      <c r="M17">
         <f>AVERAGE(Table1[FEMALE_INTEGRITY_N])</f>
-        <v>2</v>
-      </c>
-      <c r="N11">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="N17">
         <f>AVERAGE(Table1[MALE_COMPETENCE_N])</f>
-        <v>0.88888888888888884</v>
-      </c>
-      <c r="O11">
+        <v>0.6</v>
+      </c>
+      <c r="O17">
         <f>AVERAGE(Table1[MALE_BENEVOLENCE_N])</f>
-        <v>1.2222222222222223</v>
-      </c>
-      <c r="P11">
+        <v>0.93333333333333335</v>
+      </c>
+      <c r="P17">
         <f>AVERAGE(Table1[MALE_INTEGRITY_N])</f>
-        <v>1.4444444444444444</v>
+        <v>0.8</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="L15">
+  <conditionalFormatting sqref="L21">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>